<commit_message>
Fix CRDC submission test case and data sheets and data files
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/DataSubmissionValidation/DSV_TableHeaders.xlsx
+++ b/InputFiles/CRDC/DataSubmissionValidation/DSV_TableHeaders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CRDC/DataSubmissionValidation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFF0855-2E44-9442-A275-8D4718E027DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4044C6-7D15-F449-A157-268F0D83FC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="-25460" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{AF8CF42B-BA2E-1140-9C90-A27BF9CAD104}"/>
+    <workbookView xWindow="9700" yWindow="-25460" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{AF8CF42B-BA2E-1140-9C90-A27BF9CAD104}"/>
   </bookViews>
   <sheets>
     <sheet name="UploadActivities" sheetId="1" r:id="rId1"/>
@@ -67,9 +67,6 @@
     <t>Severity</t>
   </si>
   <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Expand</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>Select All</t>
+  </si>
+  <si>
+    <t>Record Count</t>
   </si>
 </sst>
 </file>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57732431-446D-0846-B624-F22E27F3F555}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,12 +542,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -559,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B8D244A-C2E7-6745-8AD5-B3D97EAFC9CF}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -570,12 +570,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -585,37 +585,37 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>